<commit_message>
thêm bộ input lấy thông tin lớp học, nhưng giấu điểm và lấy random để không lộ thông tin điểm
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,17 +459,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>24020220</t>
+          <t>24020013</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nguyễn Tiến Mạnh</t>
+          <t>Nguyễn An Quốc Anh</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3.15</t>
+          <t>3.42</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -481,20 +481,1296 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24020898</t>
+          <t>24020025</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nguyễn Văn Tính</t>
+          <t>Tạ Duy Anh</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>2.15</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>24020031</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Trần Xuân Anh</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>24020040</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Trần Việt Bảo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.94</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>24020049</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Phạm Ánh Chúc</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3.76</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>24020052</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Nguyễn Mạnh Cường</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2.63</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>24020058</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Nguyễn Hữu Danh</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.08</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>24020085</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Lưu Quang Dũng</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3.05</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>24020094</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Phạm Ngọc Dũng</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2.47</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>24021436</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Triệu Tiến Dũng</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>24020097</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Vũ Việt Dũng</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>24020107</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Trần Thùy Dương</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1.72</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>24020061</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Doãn Minh Đạt</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2.36</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>24020067</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bùi Văn Đình</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.91</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>24020073</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Cao Anh Đức</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3.11</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>24020080</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Nguyễn Ngọc Đức</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2.84</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>24020112</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Nguyễn Ngọc Trường Giang</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>24020121</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Tống Ngọc Hiển</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3.67</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>24020124</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Kiều Đăng Hiếu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.43</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>24020130</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Phan Đức Hiếu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2.28</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>24020139</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Nguyễn Hồng Hoàng</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1.96</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>24020142</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Trương Quang Hoành</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>3.54</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>24020157</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Đinh Quang Huy</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2.09</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24020166</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Phạm Lê Huy</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.78</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>24020151</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Nguyễn Trọng Hưng</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>3.21</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>24020169</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Nguyễn Trọng Khang</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>24020175</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Phạm Nam Khánh</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2.71</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>24020184</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Nguyễn Ngọc Anh Khôi</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>3.98</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>24020193</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Trịnh Tiến Kiệt</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>24020196</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Nguyễn Tuấn Lâm</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1.87</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>24020202</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Nguyễn Tuấn Linh</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2.52</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>24021555</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Nguyễn Đức Long</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>3.44</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>24020211</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Trần Bảo Long</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1.15</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>24020214</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Hoàng Xuân Lực</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2.06</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>24021558</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Ngô Thị Cẩm Ly</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>3.73</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>24020220</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Nguyễn Tiến Mạnh</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>24020229</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Kiều Nhật Minh</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>24020247</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Trần Hoài Nam</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>1.68</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>24020251</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Nguyễn Trung Nghĩa</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>3.27</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>24020256</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Nguyễn Lê Duy Nhân</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>24020265</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Phạm Công Phát</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>24020269</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Nguyễn Duy Phong</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1.24</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>24020272</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Nguyễn Ngọc Phú</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>3.62</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>24020274</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Đinh Gia Phúc</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2.18</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>23021661</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Nguyễn Hoàng Phúc</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>24020283</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Lường Tú Quân</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>3.08</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>24020292</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Đỗ Minh Sơn</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>24020301</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Cao Thị Mai Sương</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2.76</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>24020305</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Đào Quang Thái</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>3.33</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>24020310</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Triệu Tuấn Thành</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0.99</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>24020660</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Phan Văn Thuận</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2.41</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>24020319</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Thìn Thị Thúy</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>24020323</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Nguyễn Xuân Tiến</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>3.56</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>24020328</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Trần Huyền Trang</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2.04</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>24020332</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Nguyễn Huy Trọng</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0.72</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>24020337</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Nguyễn Thành Trung</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>3.19</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>24022754</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Hoàng Tạ Minh Tuấn</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>1.61</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>24020355</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Phạm Hữu Tùng</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2.88</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>24020364</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Nguyễn Hữu Vinh</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>3.47</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>24020368</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Nguyễn Lưu Vũ</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
         <is>
           <t>2</t>
         </is>

</xml_diff>